<commit_message>
4th Graph Work Finished
</commit_message>
<xml_diff>
--- a/Plot Work/1890 State Urban Population - Henry Gannett/Henry Gannett State Urban Population.xlsx
+++ b/Plot Work/1890 State Urban Population - Henry Gannett/Henry Gannett State Urban Population.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RBY11\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robby\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F364B1C1-9310-466F-98BD-E608CF8EE2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8214EE59-BF7E-4D89-A040-45F66052A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3615" windowWidth="21600" windowHeight="11835" xr2:uid="{EED4C8F8-26ED-4F17-95E9-617E89F6126D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EED4C8F8-26ED-4F17-95E9-617E89F6126D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,14 +977,14 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>389000</v>
+        <v>320000</v>
       </c>
       <c r="C29">
         <v>10177</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>378823</v>
+        <v>309823</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>